<commit_message>
PyMOL4RNA/Spliceosome_PyMOL: add csv for tracking changes
</commit_message>
<xml_diff>
--- a/rna_tools/tools/PyMOL4RNA/Spliceosome_PyMOL.xlsx
+++ b/rna_tools/tools/PyMOL4RNA/Spliceosome_PyMOL.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/magnus/work-src/rna-tools/rna_tools/tools/PyMOL4RNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2184620-81A3-984C-B08C-A6B1F6253DEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BA9013-4F1F-084C-B854-B52261C75079}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4420" windowWidth="16800" windowHeight="15840" xr2:uid="{B0D5AA2F-57A6-0240-AB4C-88455F0B20FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -3742,16 +3741,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5966D608-D48F-B244-934C-5D01D4528793}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Spliceosome_PyMOL: add yE_6n7r,	yE_6n7p
</commit_message>
<xml_diff>
--- a/rna_tools/tools/PyMOL4RNA/Spliceosome_PyMOL.xlsx
+++ b/rna_tools/tools/PyMOL4RNA/Spliceosome_PyMOL.xlsx
@@ -2,23 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/magnus/work-src/rna-tools/rna_tools/tools/PyMOL4RNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E040C68-FE59-C24A-B559-AC4152CFC6D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2681D151-9C7A-D841-825F-D44B66131E41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="27240" windowHeight="19840" xr2:uid="{B0D5AA2F-57A6-0240-AB4C-88455F0B20FF}"/>
+    <workbookView xWindow="740" yWindow="1520" windowWidth="30120" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -31,7 +34,7 @@
     <author>magnus</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{7B2A6577-99BB-CF44-B859-3E058986FEDE}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1" shapeId="0" xr:uid="{A4747542-37F0-7244-8123-C4D26CC5D33B}">
+    <comment ref="L1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -108,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1" shapeId="0" xr:uid="{AC1C5B73-7DE6-5241-BF79-0FE45B600CCE}">
+    <comment ref="M1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -136,14 +139,13 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">Cryo-EM structure of a human post-catalytic spliceosome (P complex) at 3.0 angstrom
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0" shapeId="0" xr:uid="{E3B4EE78-00C6-6940-B32B-7A08B4B219B7}">
+    <comment ref="I33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -176,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K33" authorId="0" shapeId="0" xr:uid="{A4D40821-BA50-5A4A-9CEF-4D8170799861}">
+    <comment ref="K33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -210,45 +212,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="D36" authorId="0" shapeId="0" xr:uid="{500A986F-AFC7-7349-AE96-14997BF6E7E1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Magnus:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>conclict marked</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="275">
   <si>
     <t>PRP8</t>
   </si>
@@ -484,9 +453,6 @@
     <t>Ysf3</t>
   </si>
   <si>
-    <t>exon-5</t>
-  </si>
-  <si>
     <t>exon-3</t>
   </si>
   <si>
@@ -859,9 +825,6 @@
     <t>g, n</t>
   </si>
   <si>
-    <t>unknown_unassigned</t>
-  </si>
-  <si>
     <t>b, k</t>
   </si>
   <si>
@@ -926,6 +889,159 @@
   </si>
   <si>
     <t>PRKRIP1</t>
+  </si>
+  <si>
+    <t>e,i</t>
+  </si>
+  <si>
+    <t>6bk8</t>
+  </si>
+  <si>
+    <t>5wsg</t>
+  </si>
+  <si>
+    <t>yCs_5mq0</t>
+  </si>
+  <si>
+    <t>yC_5lj5</t>
+  </si>
+  <si>
+    <t>unassigned</t>
+  </si>
+  <si>
+    <t>MUD1</t>
+  </si>
+  <si>
+    <t>SNP1</t>
+  </si>
+  <si>
+    <t>YHC1</t>
+  </si>
+  <si>
+    <t>PRP39</t>
+  </si>
+  <si>
+    <t>PRP42 (MUD16, SNU65)</t>
+  </si>
+  <si>
+    <t>NAM8 (MRE2)</t>
+  </si>
+  <si>
+    <t>SNU56 (MUD10)</t>
+  </si>
+  <si>
+    <t>LUC7 (EPE1, EXM2)</t>
+  </si>
+  <si>
+    <t>SNU71</t>
+  </si>
+  <si>
+    <t>RSE1 (SAP130)</t>
+  </si>
+  <si>
+    <t>CUS1</t>
+  </si>
+  <si>
+    <t>PRP11 (PRP10, RNA11)</t>
+  </si>
+  <si>
+    <t>PRP21 (SPP91)</t>
+  </si>
+  <si>
+    <t>b, s</t>
+  </si>
+  <si>
+    <t>d, v</t>
+  </si>
+  <si>
+    <t>e, w</t>
+  </si>
+  <si>
+    <t>f, x</t>
+  </si>
+  <si>
+    <t>g, y</t>
+  </si>
+  <si>
+    <t>h, t</t>
+  </si>
+  <si>
+    <t>i, u</t>
+  </si>
+  <si>
+    <t>yPre_6g90</t>
+  </si>
+  <si>
+    <t>grey51</t>
+  </si>
+  <si>
+    <t>grey53</t>
+  </si>
+  <si>
+    <t>grey54</t>
+  </si>
+  <si>
+    <t>grey55</t>
+  </si>
+  <si>
+    <t>grey56</t>
+  </si>
+  <si>
+    <t>grey57</t>
+  </si>
+  <si>
+    <t>grey58</t>
+  </si>
+  <si>
+    <t>grey59</t>
+  </si>
+  <si>
+    <t>grey61</t>
+  </si>
+  <si>
+    <t>grey62</t>
+  </si>
+  <si>
+    <t>grey63</t>
+  </si>
+  <si>
+    <t>grey64</t>
+  </si>
+  <si>
+    <t>grey65</t>
+  </si>
+  <si>
+    <t>grey66</t>
+  </si>
+  <si>
+    <t>grey67</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>yE_6n7r</t>
+  </si>
+  <si>
+    <t>PRP40</t>
+  </si>
+  <si>
+    <t>STO1 (CBC1, CBP80, GCR3, SUT1)</t>
+  </si>
+  <si>
+    <t>CBC2 (CBP20, MUD13, SAE1)</t>
+  </si>
+  <si>
+    <t>yE_6n7p</t>
+  </si>
+  <si>
+    <t>grey69</t>
+  </si>
+  <si>
+    <t>grey71</t>
   </si>
 </sst>
 </file>
@@ -938,7 +1054,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1021,7 +1136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1031,24 +1146,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1070,8 +1167,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1081,11 +1184,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1094,38 +1197,18 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1133,7 +1216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1207,70 +1290,50 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1585,11 +1648,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0E72E8-F810-6348-9EC2-EDEFECB8AF9D}">
-  <dimension ref="A1:P105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C91" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1607,57 +1673,78 @@
     <col min="11" max="11" width="10.83203125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>102</v>
-      </c>
       <c r="H1" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="J1" s="24" t="s">
-        <v>187</v>
-      </c>
       <c r="K1" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L1" s="24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="M1" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="N1" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="O1" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="P1" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="P1" s="31" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>225</v>
+      </c>
+      <c r="R1" t="s">
+        <v>226</v>
+      </c>
+      <c r="S1" t="s">
+        <v>227</v>
+      </c>
+      <c r="T1" t="s">
+        <v>228</v>
+      </c>
+      <c r="U1" t="s">
+        <v>250</v>
+      </c>
+      <c r="V1" t="s">
+        <v>268</v>
+      </c>
+      <c r="W1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1691,8 +1778,11 @@
       <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1716,8 +1806,11 @@
       <c r="I3" s="25"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1749,8 +1842,11 @@
       <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1758,14 +1854,14 @@
         <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>22</v>
@@ -1780,8 +1876,11 @@
       <c r="K5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1789,7 +1888,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>7</v>
@@ -1811,53 +1910,68 @@
       <c r="K6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="56">
+      <c r="T6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32">
         <v>6</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="56" t="s">
-        <v>212</v>
-      </c>
-      <c r="D7" s="57" t="s">
+      <c r="C7" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="59" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="58" t="s">
+      <c r="G7" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="58" t="s">
+      <c r="H7" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="60" t="s">
+      <c r="I7" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="56" t="s">
+      <c r="J7" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="56" t="s">
+      <c r="K7" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="61" t="s">
+      <c r="M7" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="61" t="s">
+      <c r="N7" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="61" t="s">
+      <c r="O7" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="61" t="s">
+      <c r="P7" s="37" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="R7" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="S7" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" s="37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1883,13 +1997,16 @@
         <v>24</v>
       </c>
       <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>62</v>
@@ -1922,8 +2039,14 @@
       <c r="O9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1953,8 +2076,11 @@
       <c r="K10" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1984,8 +2110,11 @@
       <c r="K11" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="T11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="17">
         <v>11</v>
       </c>
@@ -2012,16 +2141,19 @@
       <c r="O12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="P12" s="62" t="s">
+      <c r="P12" s="38" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>67</v>
@@ -2039,7 +2171,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2061,8 +2193,11 @@
       <c r="I14" s="25"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2076,7 +2211,7 @@
         <v>21</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="13" t="s">
@@ -2087,13 +2222,16 @@
         <v>29</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="U15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2107,7 +2245,7 @@
         <v>22</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="13" t="s">
@@ -2118,18 +2256,24 @@
         <v>31</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="T16" t="s">
+        <v>31</v>
+      </c>
+      <c r="U16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>61</v>
@@ -2156,13 +2300,16 @@
       <c r="K17" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>58</v>
@@ -2181,15 +2328,18 @@
         <v>32</v>
       </c>
       <c r="P18" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="T18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>65</v>
@@ -2199,14 +2349,14 @@
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J19" s="17" t="s">
         <v>25</v>
@@ -2215,12 +2365,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>71</v>
@@ -2230,21 +2380,24 @@
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="15"/>
       <c r="I20" s="27" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+      <c r="T20" s="21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2276,8 +2429,11 @@
       <c r="K21" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2309,13 +2465,16 @@
       <c r="K22" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>71</v>
@@ -2336,8 +2495,11 @@
       <c r="K23" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2371,13 +2533,16 @@
       <c r="K24" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>72</v>
@@ -2387,11 +2552,11 @@
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I25" s="25"/>
       <c r="J25" s="1" t="s">
@@ -2401,7 +2566,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2416,7 +2581,7 @@
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>26</v>
@@ -2433,356 +2598,412 @@
       <c r="K26" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="32">
+      <c r="T26" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="33" t="s">
+    </row>
+    <row r="27" spans="1:20" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="39">
+        <v>26</v>
+      </c>
+      <c r="B27" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="36">
+      <c r="F27" s="43">
         <v>2</v>
       </c>
-      <c r="G27" s="36" t="s">
+      <c r="G27" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="37">
+      <c r="H27" s="43">
         <v>2</v>
       </c>
-      <c r="I27" s="38">
+      <c r="I27" s="44">
         <v>2</v>
       </c>
-      <c r="J27" s="34" t="s">
+      <c r="J27" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="K27" s="34" t="s">
+      <c r="K27" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="L27" s="39" t="s">
+      <c r="L27" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="M27" s="39" t="s">
+      <c r="M27" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="N27" s="39">
+      <c r="N27" s="45">
         <v>2</v>
       </c>
-      <c r="O27" s="39" t="s">
+      <c r="O27" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="P27" s="39" t="s">
+      <c r="P27" s="45" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="40">
+      <c r="Q27" s="45">
+        <v>2</v>
+      </c>
+      <c r="S27" s="45">
+        <v>2</v>
+      </c>
+      <c r="T27" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="46">
         <v>27</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="13" t="s">
+      <c r="D28" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="43">
+      <c r="F28" s="50">
         <v>5</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28" s="50">
         <v>5</v>
       </c>
-      <c r="I28" s="25">
+      <c r="I28" s="51">
         <v>5</v>
       </c>
-      <c r="J28" s="28" t="s">
+      <c r="J28" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="K28" s="28" t="s">
+      <c r="K28" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="L28" s="44" t="s">
+      <c r="L28" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="M28" s="44" t="s">
+      <c r="M28" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="N28" s="44">
+      <c r="N28" s="52">
         <v>5</v>
       </c>
-      <c r="O28" s="44" t="s">
+      <c r="O28" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="P28" s="54" t="s">
+      <c r="P28" s="52" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="40">
+      <c r="Q28" s="52">
+        <v>5</v>
+      </c>
+      <c r="S28" s="52">
+        <v>5</v>
+      </c>
+      <c r="T28" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="46">
         <v>28</v>
       </c>
-      <c r="B29" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="28" t="s">
+      <c r="B29" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-    </row>
-    <row r="30" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="40">
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+    </row>
+    <row r="30" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="46">
         <v>29</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="E30" s="13" t="s">
+      <c r="D30" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="43">
+      <c r="F30" s="50">
         <v>6</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H30" s="50">
         <v>6</v>
       </c>
-      <c r="I30" s="25">
+      <c r="I30" s="51">
         <v>6</v>
       </c>
-      <c r="J30" s="28" t="s">
+      <c r="J30" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="K30" s="28" t="s">
+      <c r="K30" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="L30" s="44" t="s">
+      <c r="L30" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="M30" s="44" t="s">
+      <c r="M30" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="N30" s="44">
+      <c r="N30" s="52">
         <v>6</v>
       </c>
-      <c r="O30" s="44" t="s">
+      <c r="O30" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="P30" s="54" t="s">
+      <c r="P30" s="52" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="40"/>
-      <c r="B31" s="41" t="s">
+      <c r="Q30" s="52">
+        <v>6</v>
+      </c>
+      <c r="S30" s="52">
+        <v>6</v>
+      </c>
+      <c r="T30" s="52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="46"/>
+      <c r="B31" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="D31" s="42" t="s">
+      <c r="C31" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="D31" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="15" t="s">
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="25"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
-    </row>
-    <row r="32" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="40"/>
-      <c r="B32" s="41" t="s">
+      <c r="I31" s="51"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="S31" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="T31" s="52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="46"/>
+      <c r="B32" s="47" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="D32" s="49" t="s">
         <v>191</v>
       </c>
-      <c r="D32" s="42" t="s">
-        <v>192</v>
-      </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-    </row>
-    <row r="33" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="40">
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+    </row>
+    <row r="33" spans="1:23" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="46">
         <v>30</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="E33" s="13" t="s">
+      <c r="D33" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="E33" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F33" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="13" t="s">
+      <c r="G33" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H33" s="15" t="s">
+      <c r="H33" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="I33" s="25" t="s">
+      <c r="I33" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="J33" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="K33" s="28" t="s">
+      <c r="J33" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="K33" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="L33" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="M33" s="28" t="s">
+      <c r="L33" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="M33" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="N33" s="28" t="s">
+      <c r="N33" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="O33" s="28" t="s">
+      <c r="O33" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="P33" s="55" t="s">
+      <c r="P33" s="48" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="40">
+      <c r="Q33" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="S33" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="T33" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="V33" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="W33" s="52" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="46">
         <v>31</v>
       </c>
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="47" t="s">
+        <v>187</v>
+      </c>
+      <c r="C34" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="C34" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="D34" s="45" t="s">
-        <v>154</v>
-      </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13" t="s">
+      <c r="D34" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="G34" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="15" t="s">
+      <c r="H34" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="I34" s="25" t="s">
+      <c r="I34" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-    </row>
-    <row r="35" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="40">
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+    </row>
+    <row r="35" spans="1:23" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="46">
         <v>32</v>
       </c>
-      <c r="B35" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="C35" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="D35" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
-    </row>
-    <row r="36" spans="1:16" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="46">
-        <v>33</v>
-      </c>
-      <c r="B36" s="47" t="s">
+      <c r="B35" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="48" t="s">
-        <v>189</v>
-      </c>
-      <c r="D36" s="49" t="s">
-        <v>154</v>
-      </c>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="51"/>
-      <c r="I36" s="52"/>
-      <c r="J36" s="48"/>
-      <c r="K36" s="48"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C35" s="48" t="s">
+        <v>188</v>
+      </c>
+      <c r="D35" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="48"/>
+      <c r="S35" s="52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="14"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>147</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="13"/>
@@ -2791,21 +3012,21 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>148</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13"/>
@@ -2814,21 +3035,21 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>149</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="13"/>
@@ -2837,21 +3058,21 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>150</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>144</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="13"/>
@@ -2860,21 +3081,21 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F41" s="14"/>
       <c r="G41" s="13"/>
@@ -2883,21 +3104,21 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>152</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="13"/>
@@ -2906,21 +3127,21 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="13"/>
@@ -2929,21 +3150,21 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>98</v>
+        <v>181</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F44" s="14"/>
       <c r="G44" s="13"/>
@@ -2952,21 +3173,21 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="F45" s="14"/>
       <c r="G45" s="13"/>
@@ -2975,21 +3196,21 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>159</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>180</v>
+        <v>96</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>127</v>
+        <v>48</v>
       </c>
       <c r="F46" s="14"/>
       <c r="G46" s="13"/>
@@ -2998,21 +3219,21 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>160</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>48</v>
+        <v>142</v>
       </c>
       <c r="F47" s="14"/>
       <c r="G47" s="13"/>
@@ -3021,21 +3242,21 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>122</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>143</v>
+        <v>49</v>
       </c>
       <c r="F48" s="14"/>
       <c r="G48" s="13"/>
@@ -3044,21 +3265,21 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="F49" s="14"/>
       <c r="G49" s="13"/>
@@ -3067,70 +3288,70 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>22</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="E50" s="13"/>
       <c r="F50" s="14"/>
       <c r="G50" s="13"/>
       <c r="H50" s="15"/>
       <c r="I50" s="25"/>
-      <c r="J50" s="1"/>
+      <c r="J50" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E51" s="13"/>
-      <c r="F51" s="14"/>
+      <c r="E51" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="G51" s="13"/>
       <c r="H51" s="15"/>
       <c r="I51" s="25"/>
-      <c r="J51" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F52" s="16" t="s">
-        <v>29</v>
+        <v>171</v>
+      </c>
+      <c r="E52" s="13"/>
+      <c r="F52" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="G52" s="13"/>
       <c r="H52" s="15"/>
@@ -3138,22 +3359,24 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C53" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="E53" s="13"/>
+      <c r="E53" s="13">
+        <v>2</v>
+      </c>
       <c r="F53" s="14" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="G53" s="13"/>
       <c r="H53" s="15"/>
@@ -3161,24 +3384,22 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="E54" s="13">
-        <v>2</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="E54" s="13"/>
       <c r="F54" s="14" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="G54" s="13"/>
       <c r="H54" s="15"/>
@@ -3186,9 +3407,9 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>86</v>
@@ -3197,11 +3418,11 @@
         <v>57</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
       <c r="E55" s="13"/>
       <c r="F55" s="14" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="G55" s="13"/>
       <c r="H55" s="15"/>
@@ -3209,22 +3430,24 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E56" s="13"/>
+        <v>58</v>
+      </c>
+      <c r="D56" s="12">
+        <v>1</v>
+      </c>
+      <c r="E56" s="13">
+        <v>1</v>
+      </c>
       <c r="F56" s="14" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="G56" s="13"/>
       <c r="H56" s="15"/>
@@ -3232,24 +3455,24 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="D57" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E57" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="G57" s="13"/>
       <c r="H57" s="15"/>
@@ -3257,24 +3480,24 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="D58" s="12">
-        <v>2</v>
-      </c>
-      <c r="E58" s="13">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="G58" s="13"/>
       <c r="H58" s="15"/>
@@ -3282,24 +3505,24 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D59" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="G59" s="13"/>
       <c r="H59" s="15"/>
@@ -3307,24 +3530,22 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D60" s="12">
-        <v>4</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>92</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E60" s="13"/>
       <c r="F60" s="14" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G60" s="13"/>
       <c r="H60" s="15"/>
@@ -3332,22 +3553,24 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D61" s="12">
+        <v>6</v>
+      </c>
+      <c r="E61" s="13">
         <v>5</v>
       </c>
-      <c r="E61" s="13"/>
       <c r="F61" s="14" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G61" s="13"/>
       <c r="H61" s="15"/>
@@ -3355,24 +3578,24 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D62" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E62" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G62" s="13"/>
       <c r="H62" s="15"/>
@@ -3380,24 +3603,24 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D63" s="12">
-        <v>7</v>
-      </c>
-      <c r="E63" s="13">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G63" s="13"/>
       <c r="H63" s="15"/>
@@ -3405,68 +3628,72 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D64" s="12">
-        <v>8</v>
-      </c>
-      <c r="E64" s="13" t="s">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="E64" s="13">
+        <v>6</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="G64" s="13"/>
       <c r="H64" s="15"/>
       <c r="I64" s="25"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U64" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D65" s="12">
-        <v>9</v>
-      </c>
-      <c r="E65" s="13">
-        <v>6</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>13</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E65" s="13"/>
+      <c r="F65" s="14"/>
       <c r="G65" s="13"/>
       <c r="H65" s="15"/>
       <c r="I65" s="25"/>
-      <c r="J65" s="1"/>
+      <c r="J65" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K65" s="1"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M65" s="30" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D66" s="19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E66" s="13"/>
       <c r="F66" s="14"/>
@@ -3474,25 +3701,22 @@
       <c r="H66" s="15"/>
       <c r="I66" s="25"/>
       <c r="J66" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K66" s="1"/>
-      <c r="M66" s="30" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E67" s="13"/>
       <c r="F67" s="14"/>
@@ -3500,22 +3724,22 @@
       <c r="H67" s="15"/>
       <c r="I67" s="25"/>
       <c r="J67" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="E68" s="13"/>
       <c r="F68" s="14"/>
@@ -3523,210 +3747,292 @@
       <c r="H68" s="15"/>
       <c r="I68" s="25"/>
       <c r="J68" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:23" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D69" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="E69" s="13"/>
+      <c r="E69" s="13" t="s">
+        <v>164</v>
+      </c>
       <c r="F69" s="14"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="15"/>
-      <c r="I69" s="25"/>
+      <c r="G69" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H69" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I69" s="27" t="s">
+        <v>202</v>
+      </c>
       <c r="J69" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K69" s="1"/>
-    </row>
-    <row r="70" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="K69" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="T69" t="s">
+        <v>134</v>
+      </c>
+      <c r="U69" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="V69" t="s">
+        <v>13</v>
+      </c>
+      <c r="W69" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D70" s="19" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F70" s="14"/>
       <c r="G70" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="I70" s="27" t="s">
         <v>204</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K70" s="21" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="T70" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="U70" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="V70" t="s">
+        <v>22</v>
+      </c>
+      <c r="W70" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="E71" s="13" t="s">
         <v>168</v>
       </c>
       <c r="F71" s="14"/>
       <c r="G71" s="13" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I71" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K71" s="21" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="T71" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="U71" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="V71" t="s">
+        <v>23</v>
+      </c>
+      <c r="W71" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D72" s="19" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="E72" s="13" t="s">
         <v>169</v>
       </c>
       <c r="F72" s="14"/>
       <c r="G72" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="I72" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K72" s="21" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="T72" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="U72" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="V72" t="s">
+        <v>47</v>
+      </c>
+      <c r="W72" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D73" s="19" t="s">
-        <v>98</v>
+        <v>181</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="F73" s="14"/>
       <c r="G73" s="13" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="I73" s="27" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K73" s="21" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="T73" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="U73" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="V73" t="s">
+        <v>21</v>
+      </c>
+      <c r="W73" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D74" s="19" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F74" s="14"/>
       <c r="G74" s="13" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="I74" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>117</v>
+        <v>207</v>
+      </c>
+      <c r="J74" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="K74" s="21" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="T74" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="U74" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="V74" t="s">
+        <v>14</v>
+      </c>
+      <c r="W74" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D75" s="19" t="s">
-        <v>180</v>
+        <v>96</v>
       </c>
       <c r="E75" s="13" t="s">
         <v>166</v>
@@ -3739,57 +4045,61 @@
         <v>145</v>
       </c>
       <c r="I75" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J75" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K75" s="21" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="T75" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="U75" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="V75" t="s">
+        <v>20</v>
+      </c>
+      <c r="W75" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D76" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="E76" s="13" t="s">
-        <v>167</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="E76" s="13"/>
       <c r="F76" s="14"/>
-      <c r="G76" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="H76" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="I76" s="27" t="s">
-        <v>210</v>
-      </c>
-      <c r="J76" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="K76" s="21" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G76" s="13"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D77" s="19" t="s">
         <v>122</v>
@@ -3797,81 +4107,77 @@
       <c r="E77" s="13"/>
       <c r="F77" s="14"/>
       <c r="G77" s="13"/>
-      <c r="H77" s="15"/>
+      <c r="H77" s="15" t="s">
+        <v>84</v>
+      </c>
       <c r="I77" s="25" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="J77" s="1"/>
       <c r="K77" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D78" s="19" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="E78" s="13"/>
       <c r="F78" s="14"/>
       <c r="G78" s="13"/>
       <c r="H78" s="15" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I78" s="25" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J78" s="1"/>
       <c r="K78" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D79" s="19" t="s">
-        <v>156</v>
+        <v>89</v>
       </c>
       <c r="E79" s="13"/>
       <c r="F79" s="14"/>
       <c r="G79" s="13"/>
-      <c r="H79" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="I79" s="25" t="s">
-        <v>88</v>
-      </c>
+      <c r="H79" s="15"/>
+      <c r="I79" s="25"/>
       <c r="J79" s="1"/>
-      <c r="K79" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K79" s="1"/>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D80" s="19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E80" s="13"/>
       <c r="F80" s="14"/>
@@ -3881,20 +4187,22 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D81" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="E81" s="13"/>
+        <v>94</v>
+      </c>
+      <c r="E81" s="13" t="s">
+        <v>171</v>
+      </c>
       <c r="F81" s="14"/>
       <c r="G81" s="13"/>
       <c r="H81" s="15"/>
@@ -3902,21 +4210,21 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D82" s="19" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F82" s="14"/>
       <c r="G82" s="13"/>
@@ -3925,21 +4233,21 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D83" s="19" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>174</v>
+        <v>29</v>
       </c>
       <c r="F83" s="14"/>
       <c r="G83" s="13"/>
@@ -3948,21 +4256,21 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>175</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D84" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="E84" s="13" t="s">
-        <v>29</v>
+        <v>49</v>
+      </c>
+      <c r="E84" s="13">
+        <v>0</v>
       </c>
       <c r="F84" s="14"/>
       <c r="G84" s="13"/>
@@ -3971,21 +4279,21 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>176</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D85" s="19" t="s">
-        <v>49</v>
+        <v>173</v>
       </c>
       <c r="E85" s="13">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F85" s="14"/>
       <c r="G85" s="13"/>
@@ -3994,146 +4302,458 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>177</v>
+        <v>229</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D86" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="E86" s="13">
-        <v>9</v>
-      </c>
-      <c r="F86" s="14"/>
+        <v>182</v>
+      </c>
+      <c r="D86" s="12"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="16"/>
       <c r="G86" s="13"/>
       <c r="H86" s="15"/>
-      <c r="I86" s="25"/>
+      <c r="I86" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T86" t="s">
+        <v>126</v>
+      </c>
+      <c r="U86" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>85</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>203</v>
+        <v>86</v>
+      </c>
+      <c r="B87" s="21" t="s">
+        <v>213</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D87" s="12"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="16"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="15"/>
-      <c r="I87" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
-    </row>
-    <row r="88" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+      <c r="D87" s="7"/>
+      <c r="L87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B88" s="21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="D88" s="7"/>
       <c r="L88" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D89" s="7"/>
+      <c r="P89" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D90" s="7"/>
+      <c r="U90" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="A89" s="1">
-        <v>87</v>
-      </c>
-      <c r="B89" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D89" s="7"/>
-      <c r="L89" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="B90" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D90" s="7"/>
-      <c r="P90" t="s">
+      <c r="V90" t="s">
+        <v>5</v>
+      </c>
+      <c r="W90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D91" s="7"/>
+      <c r="U91" t="s">
+        <v>3</v>
+      </c>
+      <c r="V91" t="s">
+        <v>1</v>
+      </c>
+      <c r="W91" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D92" s="7"/>
+      <c r="U92" t="s">
+        <v>5</v>
+      </c>
+      <c r="V92" t="s">
+        <v>3</v>
+      </c>
+      <c r="W92" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D93" s="7"/>
+      <c r="U93" t="s">
+        <v>6</v>
+      </c>
+      <c r="V93" t="s">
+        <v>7</v>
+      </c>
+      <c r="W93" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D94" s="7"/>
+      <c r="U94" t="s">
+        <v>7</v>
+      </c>
+      <c r="V94" t="s">
+        <v>6</v>
+      </c>
+      <c r="W94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D95" s="7"/>
+      <c r="U95" t="s">
+        <v>8</v>
+      </c>
+      <c r="V95" t="s">
+        <v>8</v>
+      </c>
+      <c r="W95" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="B96" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D96" s="7"/>
+      <c r="U96" t="s">
+        <v>9</v>
+      </c>
+      <c r="V96" t="s">
+        <v>9</v>
+      </c>
+      <c r="W96" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="B97" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D97" s="7"/>
+      <c r="U97" t="s">
+        <v>10</v>
+      </c>
+      <c r="V97" t="s">
+        <v>11</v>
+      </c>
+      <c r="W97" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="B98" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" s="7"/>
+      <c r="U98" t="s">
+        <v>12</v>
+      </c>
+      <c r="V98" t="s">
+        <v>10</v>
+      </c>
+      <c r="W98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="B99" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D99" s="7"/>
+      <c r="U99" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
+      <c r="B100" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D100" s="7"/>
+      <c r="U100" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
+      <c r="B101" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D101" s="7"/>
+      <c r="U101" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>101</v>
+      </c>
+      <c r="B102" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D102" s="7"/>
+      <c r="U102" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>102</v>
+      </c>
+      <c r="B103" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D103" s="7"/>
+      <c r="U103" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D104" s="7"/>
+      <c r="U104" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="U105" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="U106" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>106</v>
+      </c>
+      <c r="B107" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="V107" t="s">
+        <v>24</v>
+      </c>
+      <c r="W107" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>107</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="W108" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>108</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="W109" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D91" s="7"/>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D92" s="7"/>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D93" s="7"/>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D94" s="7"/>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D95" s="7"/>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D96" s="7"/>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D97" s="7"/>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D98" s="7"/>
-    </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D99" s="7"/>
-    </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D100" s="7"/>
-    </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D101" s="7"/>
-    </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D102" s="7"/>
-    </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D103" s="7"/>
-    </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D104" s="7"/>
-    </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D105" s="7"/>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="W110" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J86">
+  <sortState ref="A2:J85">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M66" r:id="rId1" display="http://www.rcsb.org/structure/6ICZ" xr:uid="{6078B86D-54E1-4B48-B20D-E8BA710DDF8B}"/>
+    <hyperlink ref="M65" r:id="rId1" display="http://www.rcsb.org/structure/6ICZ" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>